<commit_message>
Updated crm file table
</commit_message>
<xml_diff>
--- a/CrossReferenceMatrix.xlsx
+++ b/CrossReferenceMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anura\OneDrive\Desktop\swe 2\CSITTeam011\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD70562-8EEC-4BD9-86B2-2A02B9B16110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834B435B-F3BB-4A5A-9D84-F153904E7213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6C8CA463-C179-4C1A-A2CA-8CD81262BA03}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
   <si>
     <t>Stakeholder</t>
   </si>
@@ -75,15 +75,6 @@
     <t>User Registration</t>
   </si>
   <si>
-    <t>Register New Users</t>
-  </si>
-  <si>
-    <t>User Registration Service</t>
-  </si>
-  <si>
-    <t>Registration Endpoint</t>
-  </si>
-  <si>
     <t>TC-1.1</t>
   </si>
   <si>
@@ -93,33 +84,12 @@
     <t>User Login</t>
   </si>
   <si>
-    <t>Login/Register via Google/Facebook</t>
-  </si>
-  <si>
-    <t>User Authentication Service</t>
-  </si>
-  <si>
-    <t>Login Endpoint</t>
-  </si>
-  <si>
     <t>TC-1.2</t>
   </si>
   <si>
     <t>Login with Valid Credentials</t>
   </si>
   <si>
-    <t>Real-Time Interaction</t>
-  </si>
-  <si>
-    <t>Send and Receive Messages in Real-time</t>
-  </si>
-  <si>
-    <t>Chat Management</t>
-  </si>
-  <si>
-    <t>Real-Time Messaging Endpoint</t>
-  </si>
-  <si>
     <t>TC-2</t>
   </si>
   <si>
@@ -129,54 +99,21 @@
     <t>System Admin</t>
   </si>
   <si>
-    <t>Admin Management</t>
-  </si>
-  <si>
-    <t>Manage User Accounts</t>
-  </si>
-  <si>
-    <t>User Service</t>
-  </si>
-  <si>
-    <t>User Management Endpoint</t>
-  </si>
-  <si>
     <t>TC-3</t>
   </si>
   <si>
     <t>User Management</t>
   </si>
   <si>
-    <t>Admin Content Management</t>
-  </si>
-  <si>
     <t>Manage and Create Content</t>
   </si>
   <si>
-    <t>Content Service</t>
-  </si>
-  <si>
-    <t>Content Creation Endpoint</t>
-  </si>
-  <si>
     <t>TC-4</t>
   </si>
   <si>
     <t>Content Creation</t>
   </si>
   <si>
-    <t>Notifications</t>
-  </si>
-  <si>
-    <t>Receive Notifications for Updates</t>
-  </si>
-  <si>
-    <t>Notification Service</t>
-  </si>
-  <si>
-    <t>Notification Endpoint</t>
-  </si>
-  <si>
     <t>TC-5</t>
   </si>
   <si>
@@ -189,12 +126,6 @@
     <t>Edit User Profile</t>
   </si>
   <si>
-    <t>Profile Management Service</t>
-  </si>
-  <si>
-    <t>Profile Update Endpoint</t>
-  </si>
-  <si>
     <t>TC-6</t>
   </si>
   <si>
@@ -204,18 +135,6 @@
     <t>User and System Admin</t>
   </si>
   <si>
-    <t>Admin Dashboard</t>
-  </si>
-  <si>
-    <t>View and Monitor App Activity</t>
-  </si>
-  <si>
-    <t>Dashboard Service</t>
-  </si>
-  <si>
-    <t>Dashboard Data Endpoint</t>
-  </si>
-  <si>
     <t>TC-7</t>
   </si>
   <si>
@@ -225,49 +144,109 @@
     <t>User Deactivation</t>
   </si>
   <si>
-    <t>Deactivate User Accounts</t>
-  </si>
-  <si>
-    <t>Admin Service</t>
-  </si>
-  <si>
-    <t>Deactivate User Endpoint</t>
-  </si>
-  <si>
     <t>TC-8</t>
   </si>
   <si>
-    <t>Event Creation</t>
-  </si>
-  <si>
-    <t>Create and Join Events</t>
-  </si>
-  <si>
-    <t>Event Service</t>
-  </si>
-  <si>
-    <t>Event Management Endpoint</t>
-  </si>
-  <si>
-    <t>TC-9</t>
-  </si>
-  <si>
-    <t>Secure Authentication</t>
-  </si>
-  <si>
-    <t>Implement Secure Login (OAuth 2.0, JWT)</t>
-  </si>
-  <si>
     <t>Authentication Service</t>
   </si>
   <si>
-    <t>Secure Authentication Endpoint</t>
-  </si>
-  <si>
-    <t>TC-10</t>
-  </si>
-  <si>
-    <t>Secure Login Test</t>
+    <t>User Authentication</t>
+  </si>
+  <si>
+    <t>Portfolio Management</t>
+  </si>
+  <si>
+    <t>Market Data Visualization</t>
+  </si>
+  <si>
+    <t>Security Threats</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>Investment Tracking</t>
+  </si>
+  <si>
+    <t>Core Security Features</t>
+  </si>
+  <si>
+    <t>Stock Search and Information</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Performance Analysis</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>1. System Context Diagram</t>
+  </si>
+  <si>
+    <t>2. Container Diagram</t>
+  </si>
+  <si>
+    <t>3. Component Diagram</t>
+  </si>
+  <si>
+    <t>4. Deployment Diagram</t>
+  </si>
+  <si>
+    <t>User Interactions</t>
+  </si>
+  <si>
+    <t>Frontend/Backend Components</t>
+  </si>
+  <si>
+    <t>Portfolio Service</t>
+  </si>
+  <si>
+    <t>Market Data Service</t>
+  </si>
+  <si>
+    <t>Backend Service</t>
+  </si>
+  <si>
+    <t>AWS Cloud Security</t>
+  </si>
+  <si>
+    <t>Transaction Service</t>
+  </si>
+  <si>
+    <t>Authentication Component</t>
+  </si>
+  <si>
+    <t>Stock Data Service</t>
+  </si>
+  <si>
+    <t>User Interface Design Guidelines</t>
+  </si>
+  <si>
+    <t>Data Protection</t>
+  </si>
+  <si>
+    <t>Key Screens</t>
+  </si>
+  <si>
+    <t>Optimization Strategies</t>
+  </si>
+  <si>
+    <t>Error Management</t>
   </si>
 </sst>
 </file>
@@ -628,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95613846-276C-4174-B8A5-AF2DFD7508D7}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,175 +667,175 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>4.0999999999999996</v>
+      <c r="B2" t="s">
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2">
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2">
+        <v>3.1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2">
-        <v>6.1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>4.0999999999999996</v>
+      <c r="B3" t="s">
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>4.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="H3">
-        <v>6.1</v>
+        <v>3.1</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>4.3</v>
+      <c r="B4" t="s">
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D4">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="H4">
-        <v>6.2</v>
+        <v>3.2</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D5">
-        <v>4.3</v>
+        <v>3.1</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5">
-        <v>2.2000000000000002</v>
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H5">
-        <v>6.3</v>
+        <v>3.3</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>4.5999999999999996</v>
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>4.4000000000000004</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6">
-        <v>2.2000000000000002</v>
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="H6">
-        <v>6.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -867,31 +846,31 @@
         <v>3.2</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D7">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H7">
-        <v>6.5</v>
+        <v>5.2</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -899,171 +878,104 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>2.2999999999999998</v>
+        <v>5.2</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>4.5999999999999996</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H8">
-        <v>6.6</v>
+        <v>4.2</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>3.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
         <v>55</v>
       </c>
-      <c r="B9">
-        <v>4.7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9">
-        <v>4.7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9">
-        <v>2.2999999999999998</v>
-      </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H9">
-        <v>6.7</v>
+        <v>6.1</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10">
-        <v>4.5999999999999996</v>
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <v>6.1</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10">
-        <v>3.2</v>
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="H10">
-        <v>6.8</v>
+        <v>7.1</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>4.2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11">
-        <v>4.8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11">
-        <v>6.9</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12">
-        <v>6.1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" t="s">
-        <v>76</v>
-      </c>
-      <c r="K12" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>